<commit_message>
Added timings for fast upgma algorithm
</commit_message>
<xml_diff>
--- a/AlgorithmTimings.xlsx
+++ b/AlgorithmTimings.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t>WPGMA</t>
   </si>
@@ -375,15 +375,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
@@ -665,56 +665,130 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>9</v>
       </c>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
+      <c r="B28" s="1">
+        <v>53197</v>
+      </c>
+      <c r="C28" s="1">
+        <v>2409</v>
+      </c>
+      <c r="D28" s="1">
+        <v>973</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
+      <c r="B29" s="1">
+        <v>53321</v>
+      </c>
+      <c r="C29" s="1">
+        <v>2412</v>
+      </c>
+      <c r="D29" s="1">
+        <v>975</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
+      <c r="B30" s="1">
+        <v>53507</v>
+      </c>
+      <c r="C30" s="1">
+        <v>2376</v>
+      </c>
+      <c r="D30" s="1">
+        <v>991</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
+      <c r="B31" s="1">
+        <v>53110</v>
+      </c>
+      <c r="C31" s="1">
+        <v>2394</v>
+      </c>
+      <c r="D31" s="1">
+        <v>968</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
+      <c r="B32" s="1">
+        <v>53411</v>
+      </c>
+      <c r="C32" s="1">
+        <v>2341</v>
+      </c>
+      <c r="D32" s="1">
+        <v>973</v>
+      </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
+      <c r="B33" s="1">
+        <v>53292</v>
+      </c>
+      <c r="C33" s="1">
+        <v>2419</v>
+      </c>
+      <c r="D33" s="1">
+        <v>983</v>
+      </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
+      <c r="B34" s="1">
+        <v>53240</v>
+      </c>
+      <c r="C34" s="1">
+        <v>2442</v>
+      </c>
+      <c r="D34" s="1">
+        <v>959</v>
+      </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
+      <c r="B35" s="1">
+        <v>53248</v>
+      </c>
+      <c r="C35" s="1">
+        <v>2477</v>
+      </c>
+      <c r="D35" s="1">
+        <v>969</v>
+      </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
+      <c r="B36" s="1">
+        <v>53405</v>
+      </c>
+      <c r="C36" s="1">
+        <v>2469</v>
+      </c>
+      <c r="D36" s="1">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="1">
+        <v>53462</v>
+      </c>
+      <c r="C37" s="1">
+        <v>2386</v>
+      </c>
+      <c r="D37" s="1">
+        <v>949</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Generated diagram of speed measurements
</commit_message>
<xml_diff>
--- a/AlgorithmTimings.xlsx
+++ b/AlgorithmTimings.xlsx
@@ -12,7 +12,9 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="FullData" sheetId="1" r:id="rId1"/>
+    <sheet name="Summary" sheetId="2" r:id="rId2"/>
+    <sheet name="SummaryDiagram" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
   <si>
     <t>WPGMA</t>
   </si>
@@ -55,13 +57,38 @@
   <si>
     <t>Fast UPGMA</t>
   </si>
+  <si>
+    <t>scince then:</t>
+  </si>
+  <si>
+    <t>Update memory usage: overwriting old distances (caching no longer needs longer matrix)</t>
+  </si>
+  <si>
+    <t>Change to x64</t>
+  </si>
+  <si>
+    <t>(Weimar, 10 Clusters, modified: yes)</t>
+  </si>
+  <si>
+    <t>Weimar, 10 Clusters, modified output</t>
+  </si>
+  <si>
+    <t>UPGMA (without distance caching)</t>
+  </si>
+  <si>
+    <t>UPGMA (fast / cached distances)</t>
+  </si>
+  <si>
+    <t>WPGMA (fast / cached distances)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0&quot; ms&quot;"/>
+    <numFmt numFmtId="165" formatCode="#,##0&quot; ms&quot;"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -92,9 +119,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -110,6 +138,1269 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-CH"/>
+              <a:t>Speed</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="de-CH" baseline="0"/>
+              <a:t> Measurements - Hierarchical Clustering  - Weimar</a:t>
+            </a:r>
+            <a:endParaRPr lang="de-CH"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Summary!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>UPGMA (without distance caching)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Summary!$B$3:$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Floyd-Warshall</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>All Pairs Dijkstra</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>All Pairs Dijkstra, parallel 4 cores</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Summary!$B$4:$D$4</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0" ms"</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>98776.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>62052.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>61515.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Summary!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>UPGMA (fast / cached distances)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="-1800000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Summary!$B$3:$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Floyd-Warshall</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>All Pairs Dijkstra</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>All Pairs Dijkstra, parallel 4 cores</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Summary!$B$5:$D$5</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0" ms"</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>15084.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2119.8000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>858.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Summary!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>WPGMA (fast / cached distances)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="-1800000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Summary!$B$3:$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Floyd-Warshall</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>All Pairs Dijkstra</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>All Pairs Dijkstra, parallel 4 cores</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Summary!$B$6:$D$6</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0" ms"</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>15104.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2105.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>846.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="-1515790512"/>
+        <c:axId val="-1515787792"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-1515790512"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1515787792"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-1515787792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-CH"/>
+                  <a:t>Measured Time</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0&quot; ms&quot;" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1515790512"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="136" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="11" orientation="landscape" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</chartsheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="6177243" cy="3774982"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -375,10 +1666,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:F69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -517,281 +1808,657 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B13" s="1">
         <v>39680</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C13" s="1">
         <v>2697</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D13" s="1">
         <v>1155</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="1">
-        <v>39514</v>
-      </c>
-      <c r="C13" s="1">
-        <v>2564</v>
-      </c>
-      <c r="D13" s="1">
-        <v>1141</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
-        <v>39594</v>
+        <v>39514</v>
       </c>
       <c r="C14" s="1">
-        <v>2616</v>
+        <v>2564</v>
       </c>
       <c r="D14" s="1">
-        <v>1048</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
-        <v>39916</v>
+        <v>39594</v>
       </c>
       <c r="C15" s="1">
-        <v>2597</v>
+        <v>2616</v>
       </c>
       <c r="D15" s="1">
-        <v>1090</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
+        <v>39916</v>
+      </c>
+      <c r="C16" s="1">
+        <v>2597</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="1">
         <v>39640</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C17" s="1">
         <v>2641</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D17" s="1">
         <v>1069</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="1">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="1">
         <v>39551</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C18" s="1">
         <v>2602</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D18" s="1">
         <v>1058</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="1">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="1">
         <v>39528</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C19" s="1">
         <v>2618</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D19" s="1">
         <v>1073</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="1">
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="1">
         <v>39619</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C20" s="1">
         <v>2606</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D20" s="1">
         <v>1078</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="1">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="1">
         <v>39631</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C21" s="1">
         <v>2565</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D21" s="1">
         <v>1049</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="1">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="1">
         <v>39839</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C22" s="1">
         <v>2575</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D22" s="1">
         <v>1071</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>6</v>
-      </c>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>8</v>
+      </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>5</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>2</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C28" t="s">
         <v>3</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D28" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>9</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B29" s="1">
         <v>53197</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C29" s="1">
         <v>2409</v>
       </c>
-      <c r="D28" s="1">
+      <c r="D29" s="1">
         <v>973</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="1">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B30" s="1">
         <v>53321</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C30" s="1">
         <v>2412</v>
       </c>
-      <c r="D29" s="1">
+      <c r="D30" s="1">
         <v>975</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="1">
         <v>53507</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C31" s="1">
         <v>2376</v>
       </c>
-      <c r="D30" s="1">
+      <c r="D31" s="1">
         <v>991</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B31" s="1">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B32" s="1">
         <v>53110</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C32" s="1">
         <v>2394</v>
       </c>
-      <c r="D31" s="1">
+      <c r="D32" s="1">
         <v>968</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B32" s="1">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B33" s="1">
         <v>53411</v>
       </c>
-      <c r="C32" s="1">
+      <c r="C33" s="1">
         <v>2341</v>
       </c>
-      <c r="D32" s="1">
+      <c r="D33" s="1">
         <v>973</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B34" s="1">
         <v>53292</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C34" s="1">
         <v>2419</v>
       </c>
-      <c r="D33" s="1">
+      <c r="D34" s="1">
         <v>983</v>
       </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B34" s="1">
+      <c r="F34" s="1"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B35" s="1">
         <v>53240</v>
       </c>
-      <c r="C34" s="1">
+      <c r="C35" s="1">
         <v>2442</v>
       </c>
-      <c r="D34" s="1">
+      <c r="D35" s="1">
         <v>959</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B35" s="1">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B36" s="1">
         <v>53248</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C36" s="1">
         <v>2477</v>
       </c>
-      <c r="D35" s="1">
+      <c r="D36" s="1">
         <v>969</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B36" s="1">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B37" s="1">
         <v>53405</v>
       </c>
-      <c r="C36" s="1">
+      <c r="C37" s="1">
         <v>2469</v>
       </c>
-      <c r="D36" s="1">
+      <c r="D37" s="1">
         <v>974</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B37" s="1">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B38" s="1">
         <v>53462</v>
       </c>
-      <c r="C37" s="1">
+      <c r="C38" s="1">
         <v>2386</v>
       </c>
-      <c r="D37" s="1">
+      <c r="D38" s="1">
         <v>949</v>
       </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>13</v>
+      </c>
+      <c r="B44" t="s">
+        <v>2</v>
+      </c>
+      <c r="C44" t="s">
+        <v>3</v>
+      </c>
+      <c r="D44" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>9</v>
+      </c>
+      <c r="B45" s="1">
+        <v>15122</v>
+      </c>
+      <c r="C45" s="1">
+        <v>2172</v>
+      </c>
+      <c r="D45" s="1">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B46" s="1">
+        <v>15240</v>
+      </c>
+      <c r="C46" s="1">
+        <v>2124</v>
+      </c>
+      <c r="D46" s="1">
+        <v>852</v>
+      </c>
+      <c r="F46" s="1"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B47" s="1">
+        <v>15005</v>
+      </c>
+      <c r="C47" s="1">
+        <v>2135</v>
+      </c>
+      <c r="D47" s="1">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B48" s="1">
+        <v>14920</v>
+      </c>
+      <c r="C48" s="1">
+        <v>2126</v>
+      </c>
+      <c r="D48" s="1">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B49" s="1">
+        <v>15006</v>
+      </c>
+      <c r="C49" s="1">
+        <v>2132</v>
+      </c>
+      <c r="D49" s="1">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B50" s="1">
+        <v>15033</v>
+      </c>
+      <c r="C50" s="1">
+        <v>2107</v>
+      </c>
+      <c r="D50" s="1">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B51" s="1">
+        <v>15053</v>
+      </c>
+      <c r="C51" s="1">
+        <v>2101</v>
+      </c>
+      <c r="D51" s="1">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B52" s="1">
+        <v>15099</v>
+      </c>
+      <c r="C52" s="1">
+        <v>2117</v>
+      </c>
+      <c r="D52" s="1">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B53" s="1">
+        <v>15188</v>
+      </c>
+      <c r="C53" s="1">
+        <v>2089</v>
+      </c>
+      <c r="D53" s="1">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B54" s="1">
+        <v>15178</v>
+      </c>
+      <c r="C54" s="1">
+        <v>2095</v>
+      </c>
+      <c r="D54" s="1">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>0</v>
+      </c>
+      <c r="B56" s="1">
+        <v>15012</v>
+      </c>
+      <c r="C56" s="1">
+        <v>2091</v>
+      </c>
+      <c r="D56" s="1">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B57" s="1">
+        <v>15036</v>
+      </c>
+      <c r="C57" s="1">
+        <v>2086</v>
+      </c>
+      <c r="D57" s="1">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B58" s="1">
+        <v>15179</v>
+      </c>
+      <c r="C58" s="1">
+        <v>2117</v>
+      </c>
+      <c r="D58" s="1">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B59" s="1">
+        <v>15152</v>
+      </c>
+      <c r="C59" s="1">
+        <v>2123</v>
+      </c>
+      <c r="D59" s="1">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B60" s="1">
+        <v>15135</v>
+      </c>
+      <c r="C60" s="1">
+        <v>2075</v>
+      </c>
+      <c r="D60" s="1">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B61" s="1">
+        <v>15239</v>
+      </c>
+      <c r="C61" s="1">
+        <v>2122</v>
+      </c>
+      <c r="D61" s="1">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B62" s="1">
+        <v>15074</v>
+      </c>
+      <c r="C62" s="1">
+        <v>2168</v>
+      </c>
+      <c r="D62" s="1">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B63" s="1">
+        <v>15065</v>
+      </c>
+      <c r="C63" s="1">
+        <v>2108</v>
+      </c>
+      <c r="D63" s="1">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B64" s="1">
+        <v>15099</v>
+      </c>
+      <c r="C64" s="1">
+        <v>2062</v>
+      </c>
+      <c r="D64" s="1">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B65" s="1">
+        <v>15051</v>
+      </c>
+      <c r="C65" s="1">
+        <v>2107</v>
+      </c>
+      <c r="D65" s="1">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B66" s="1"/>
+      <c r="C66" s="1"/>
+      <c r="D66" s="1"/>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B67" s="1"/>
+      <c r="C67" s="1"/>
+      <c r="D67" s="1"/>
+    </row>
+    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B68" s="1"/>
+      <c r="C68" s="1"/>
+      <c r="D68" s="1"/>
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B69" s="1"/>
+      <c r="C69" s="1"/>
+      <c r="D69" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="2">
+        <f>AVERAGE(FullData!B2:B11)</f>
+        <v>98776.2</v>
+      </c>
+      <c r="C4" s="2">
+        <f>AVERAGE(FullData!C2:C11)</f>
+        <v>62052.1</v>
+      </c>
+      <c r="D4" s="2">
+        <f>AVERAGE(FullData!D2:D11)</f>
+        <v>61515.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="2">
+        <f>AVERAGE(FullData!B45:B54)</f>
+        <v>15084.4</v>
+      </c>
+      <c r="C5" s="2">
+        <f>AVERAGE(FullData!C45:C54)</f>
+        <v>2119.8000000000002</v>
+      </c>
+      <c r="D5" s="2">
+        <f>AVERAGE(FullData!D45:D54)</f>
+        <v>858.7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="2">
+        <f>AVERAGE(FullData!B56:B65)</f>
+        <v>15104.2</v>
+      </c>
+      <c r="C6" s="2">
+        <f>AVERAGE(FullData!C56:C65)</f>
+        <v>2105.9</v>
+      </c>
+      <c r="D6" s="2">
+        <f>AVERAGE(FullData!D56:D65)</f>
+        <v>846.1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Created speed measurements for kmeans
</commit_message>
<xml_diff>
--- a/AlgorithmTimings.xlsx
+++ b/AlgorithmTimings.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="FullData" sheetId="1" r:id="rId1"/>
     <sheet name="Summary" sheetId="2" r:id="rId2"/>
     <sheet name="SummaryDiagram" sheetId="3" r:id="rId3"/>
+    <sheet name="KMeansDiagram" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
   <si>
     <t>WPGMA</t>
   </si>
@@ -80,6 +81,24 @@
   </si>
   <si>
     <t>WPGMA (fast / cached distances)</t>
+  </si>
+  <si>
+    <t>K-Means</t>
+  </si>
+  <si>
+    <t>Original</t>
+  </si>
+  <si>
+    <t>Parallel</t>
+  </si>
+  <si>
+    <t>Shortest Path</t>
+  </si>
+  <si>
+    <t>Parallel &amp; Shortest Path</t>
+  </si>
+  <si>
+    <t>Original &amp; Shortest Path</t>
   </si>
 </sst>
 </file>
@@ -586,11 +605,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-1515790512"/>
-        <c:axId val="-1515787792"/>
+        <c:axId val="-874014784"/>
+        <c:axId val="-874004992"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1515790512"/>
+        <c:axId val="-874014784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -633,7 +652,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1515787792"/>
+        <c:crossAx val="-874004992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -641,7 +660,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1515787792"/>
+        <c:axId val="-874004992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -748,7 +767,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1515790512"/>
+        <c:crossAx val="-874014784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -824,6 +843,414 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-CH"/>
+              <a:t>Speed Measurements - K-Means - Weimar</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Summary!$B$8:$E$8</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Original</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Original &amp; Shortest Path</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Parallel</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Parallel &amp; Shortest Path</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Summary!$B$9:$E$9</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0" ms"</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>29175.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32162.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16810.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17704.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="-773344848"/>
+        <c:axId val="-773349744"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-773344848"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-773349744"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-773349744"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-CH"/>
+                  <a:t>Measured Time</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0&quot; ms&quot;" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-773344848"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
   <a:schemeClr val="accent2"/>
@@ -861,6 +1288,43 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+  <a:schemeClr val="accent6"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent4"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -1364,11 +1828,526 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="136" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="187" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="11" orientation="landscape" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="187" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="11" orientation="landscape" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -1378,9 +2357,79 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>437809</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>142549</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Grafik 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7572375" y="12582525"/>
+          <a:ext cx="2723809" cy="2609524"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="6177243" cy="3774982"/>
+    <xdr:ext cx="6183610" cy="3779439"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="6168329" cy="3779439"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Diagramm 1"/>
@@ -1666,10 +2715,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F69"/>
+  <dimension ref="A1:F98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1678,6 +2727,7 @@
     <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -2338,7 +3388,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B65" s="1">
         <v>15051</v>
       </c>
@@ -2349,38 +3399,307 @@
         <v>869</v>
       </c>
     </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
     </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B67" s="1"/>
-      <c r="C67" s="1"/>
-      <c r="D67" s="1"/>
-    </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B68" s="1"/>
-      <c r="C68" s="1"/>
-      <c r="D68" s="1"/>
-    </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B69" s="1"/>
-      <c r="C69" s="1"/>
-      <c r="D69" s="1"/>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>18</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B68" s="1">
+        <v>29628</v>
+      </c>
+      <c r="C68" s="1">
+        <v>16104</v>
+      </c>
+      <c r="D68" s="1">
+        <v>33106</v>
+      </c>
+      <c r="E68" s="1">
+        <v>16838</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B69" s="1">
+        <v>28633</v>
+      </c>
+      <c r="C69" s="1">
+        <v>16268</v>
+      </c>
+      <c r="D69" s="1">
+        <v>31312</v>
+      </c>
+      <c r="E69" s="1">
+        <v>17135</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B70" s="1">
+        <v>28894</v>
+      </c>
+      <c r="C70" s="1">
+        <v>15959</v>
+      </c>
+      <c r="D70" s="1">
+        <v>31382</v>
+      </c>
+      <c r="E70" s="1">
+        <v>18046</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B71" s="1">
+        <v>29374</v>
+      </c>
+      <c r="C71" s="1">
+        <v>16149</v>
+      </c>
+      <c r="D71" s="1">
+        <v>32998</v>
+      </c>
+      <c r="E71" s="1">
+        <v>17590</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B72" s="1">
+        <v>29027</v>
+      </c>
+      <c r="C72" s="1">
+        <v>17704</v>
+      </c>
+      <c r="D72" s="1">
+        <v>32108</v>
+      </c>
+      <c r="E72" s="1">
+        <v>17991</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B73" s="1">
+        <v>28969</v>
+      </c>
+      <c r="C73" s="1">
+        <v>15937</v>
+      </c>
+      <c r="D73" s="1">
+        <v>32251</v>
+      </c>
+      <c r="E73" s="1">
+        <v>17923</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B74" s="1">
+        <v>28954</v>
+      </c>
+      <c r="C74" s="1">
+        <v>18308</v>
+      </c>
+      <c r="D74" s="1">
+        <v>32158</v>
+      </c>
+      <c r="E74" s="1">
+        <v>17291</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B75" s="1">
+        <v>29060</v>
+      </c>
+      <c r="C75" s="1">
+        <v>16462</v>
+      </c>
+      <c r="D75" s="1">
+        <v>31480</v>
+      </c>
+      <c r="E75" s="1">
+        <v>17132</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B76" s="1">
+        <v>30612</v>
+      </c>
+      <c r="C76" s="1">
+        <v>16756</v>
+      </c>
+      <c r="D76" s="1">
+        <v>33418</v>
+      </c>
+      <c r="E76" s="1">
+        <v>18817</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B77" s="1">
+        <v>28604</v>
+      </c>
+      <c r="C77" s="1">
+        <v>18461</v>
+      </c>
+      <c r="D77" s="1">
+        <v>31413</v>
+      </c>
+      <c r="E77" s="1">
+        <v>18280</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B78" s="1"/>
+      <c r="C78" s="1"/>
+      <c r="D78" s="1"/>
+      <c r="E78" s="1"/>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B79" s="1"/>
+      <c r="C79" s="1"/>
+      <c r="D79" s="1"/>
+      <c r="E79" s="1"/>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B80" s="1"/>
+      <c r="C80" s="1"/>
+      <c r="D80" s="1"/>
+      <c r="E80" s="1"/>
+    </row>
+    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B81" s="1"/>
+      <c r="C81" s="1"/>
+      <c r="D81" s="1"/>
+      <c r="E81" s="1"/>
+    </row>
+    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B82" s="1"/>
+      <c r="C82" s="1"/>
+      <c r="D82" s="1"/>
+      <c r="E82" s="1"/>
+    </row>
+    <row r="83" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B83" s="1"/>
+      <c r="C83" s="1"/>
+      <c r="D83" s="1"/>
+      <c r="E83" s="1"/>
+    </row>
+    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B84" s="1"/>
+      <c r="C84" s="1"/>
+      <c r="D84" s="1"/>
+      <c r="E84" s="1"/>
+    </row>
+    <row r="85" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B85" s="1"/>
+      <c r="C85" s="1"/>
+      <c r="D85" s="1"/>
+      <c r="E85" s="1"/>
+    </row>
+    <row r="86" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B86" s="1"/>
+      <c r="C86" s="1"/>
+      <c r="D86" s="1"/>
+      <c r="E86" s="1"/>
+    </row>
+    <row r="87" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B87" s="1"/>
+      <c r="C87" s="1"/>
+      <c r="D87" s="1"/>
+      <c r="E87" s="1"/>
+    </row>
+    <row r="88" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B88" s="1"/>
+      <c r="C88" s="1"/>
+      <c r="D88" s="1"/>
+      <c r="E88" s="1"/>
+    </row>
+    <row r="89" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B89" s="1"/>
+      <c r="C89" s="1"/>
+      <c r="D89" s="1"/>
+      <c r="E89" s="1"/>
+    </row>
+    <row r="90" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B90" s="1"/>
+      <c r="C90" s="1"/>
+      <c r="D90" s="1"/>
+      <c r="E90" s="1"/>
+    </row>
+    <row r="91" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B91" s="1"/>
+      <c r="C91" s="1"/>
+      <c r="D91" s="1"/>
+      <c r="E91" s="1"/>
+    </row>
+    <row r="92" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B92" s="1"/>
+      <c r="C92" s="1"/>
+      <c r="D92" s="1"/>
+      <c r="E92" s="1"/>
+    </row>
+    <row r="93" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B93" s="1"/>
+      <c r="C93" s="1"/>
+      <c r="D93" s="1"/>
+      <c r="E93" s="1"/>
+    </row>
+    <row r="94" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B94" s="1"/>
+      <c r="C94" s="1"/>
+      <c r="D94" s="1"/>
+      <c r="E94" s="1"/>
+    </row>
+    <row r="95" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B95" s="1"/>
+      <c r="C95" s="1"/>
+      <c r="D95" s="1"/>
+      <c r="E95" s="1"/>
+    </row>
+    <row r="96" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B96" s="1"/>
+      <c r="C96" s="1"/>
+      <c r="D96" s="1"/>
+      <c r="E96" s="1"/>
+    </row>
+    <row r="97" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B97" s="1"/>
+      <c r="C97" s="1"/>
+      <c r="D97" s="1"/>
+      <c r="E97" s="1"/>
+    </row>
+    <row r="98" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B98" s="1"/>
+      <c r="C98" s="1"/>
+      <c r="D98" s="1"/>
+      <c r="E98" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:D6"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2389,14 +3708,15 @@
     <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>2</v>
       </c>
@@ -2407,7 +3727,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -2424,7 +3744,7 @@
         <v>61515.8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -2441,7 +3761,7 @@
         <v>858.7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -2456,6 +3776,41 @@
       <c r="D6" s="2">
         <f>AVERAGE(FullData!D56:D65)</f>
         <v>846.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="2">
+        <f>AVERAGE(FullData!B68:B77)</f>
+        <v>29175.5</v>
+      </c>
+      <c r="C9" s="2">
+        <f>AVERAGE(FullData!D68:D77)</f>
+        <v>32162.6</v>
+      </c>
+      <c r="D9" s="2">
+        <f>AVERAGE(FullData!C68:C77)</f>
+        <v>16810.8</v>
+      </c>
+      <c r="E9" s="2">
+        <f>AVERAGE(FullData!E68:E77)</f>
+        <v>17704.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished speed measurement section
</commit_message>
<xml_diff>
--- a/AlgorithmTimings.xlsx
+++ b/AlgorithmTimings.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="FullData" sheetId="1" r:id="rId1"/>
@@ -246,11 +246,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Summary!$A$4</c:f>
+              <c:f>Summary!$B$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>UPGMA (without distance caching)</c:v>
+                  <c:v>Floyd-Warshall</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -325,24 +325,24 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Summary!$B$3:$D$3</c:f>
+              <c:f>Summary!$A$4:$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>Floyd-Warshall</c:v>
+                  <c:v>UPGMA (without distance caching)</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>All Pairs Dijkstra</c:v>
+                  <c:v>UPGMA (fast / cached distances)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>All Pairs Dijkstra, parallel 4 cores</c:v>
+                  <c:v>WPGMA (fast / cached distances)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Summary!$B$4:$D$4</c:f>
+              <c:f>Summary!$B$4:$B$6</c:f>
               <c:numCache>
                 <c:formatCode>#,##0" ms"</c:formatCode>
                 <c:ptCount val="3"/>
@@ -350,10 +350,10 @@
                   <c:v>98776.2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>62052.1</c:v>
+                  <c:v>15084.4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>61515.8</c:v>
+                  <c:v>15104.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -364,11 +364,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Summary!$A$5</c:f>
+              <c:f>Summary!$C$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>UPGMA (fast / cached distances)</c:v>
+                  <c:v>All Pairs Dijkstra</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -443,35 +443,35 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Summary!$B$3:$D$3</c:f>
+              <c:f>Summary!$A$4:$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>Floyd-Warshall</c:v>
+                  <c:v>UPGMA (without distance caching)</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>All Pairs Dijkstra</c:v>
+                  <c:v>UPGMA (fast / cached distances)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>All Pairs Dijkstra, parallel 4 cores</c:v>
+                  <c:v>WPGMA (fast / cached distances)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Summary!$B$5:$D$5</c:f>
+              <c:f>Summary!$C$4:$C$6</c:f>
               <c:numCache>
                 <c:formatCode>#,##0" ms"</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>15084.4</c:v>
+                  <c:v>62052.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2119.8000000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>858.7</c:v>
+                  <c:v>2105.9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -482,11 +482,11 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Summary!$A$6</c:f>
+              <c:f>Summary!$D$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>WPGMA (fast / cached distances)</c:v>
+                  <c:v>All Pairs Dijkstra, parallel 4 cores</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -531,7 +531,6 @@
                 <a:endParaRPr lang="de-DE"/>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -562,32 +561,32 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Summary!$B$3:$D$3</c:f>
+              <c:f>Summary!$A$4:$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>Floyd-Warshall</c:v>
+                  <c:v>UPGMA (without distance caching)</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>All Pairs Dijkstra</c:v>
+                  <c:v>UPGMA (fast / cached distances)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>All Pairs Dijkstra, parallel 4 cores</c:v>
+                  <c:v>WPGMA (fast / cached distances)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Summary!$B$6:$D$6</c:f>
+              <c:f>Summary!$D$4:$D$6</c:f>
               <c:numCache>
                 <c:formatCode>#,##0" ms"</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>15104.2</c:v>
+                  <c:v>61515.8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2105.9</c:v>
+                  <c:v>858.7</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>846.1</c:v>
@@ -605,11 +604,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-874014784"/>
-        <c:axId val="-874004992"/>
+        <c:axId val="-1886015600"/>
+        <c:axId val="-1886019952"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-874014784"/>
+        <c:axId val="-1886015600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -652,7 +651,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-874004992"/>
+        <c:crossAx val="-1886019952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -660,7 +659,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-874004992"/>
+        <c:axId val="-1886019952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -767,7 +766,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-874014784"/>
+        <c:crossAx val="-1886015600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1045,11 +1044,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-773344848"/>
-        <c:axId val="-773349744"/>
+        <c:axId val="-1886019408"/>
+        <c:axId val="-1886018864"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-773344848"/>
+        <c:axId val="-1886019408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1092,7 +1091,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-773349744"/>
+        <c:crossAx val="-1886018864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1100,7 +1099,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-773349744"/>
+        <c:axId val="-1886018864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1207,7 +1206,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-773344848"/>
+        <c:crossAx val="-1886019408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2335,7 +2334,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="187" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="187" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="11" orientation="landscape" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -2347,7 +2346,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="187" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="136" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="11" orientation="landscape" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -2402,7 +2401,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="6183610" cy="3779439"/>
+    <xdr:ext cx="6177243" cy="3774982"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Diagramm 1"/>
@@ -2429,7 +2428,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="6168329" cy="3779439"/>
+    <xdr:ext cx="6177243" cy="3774982"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Diagramm 1"/>

</xml_diff>

<commit_message>
Added speed measurements tables
</commit_message>
<xml_diff>
--- a/AlgorithmTimings.xlsx
+++ b/AlgorithmTimings.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835"/>
   </bookViews>
   <sheets>
     <sheet name="FullData" sheetId="1" r:id="rId1"/>
@@ -604,11 +604,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-1886015600"/>
-        <c:axId val="-1886019952"/>
+        <c:axId val="1523426784"/>
+        <c:axId val="1523418624"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1886015600"/>
+        <c:axId val="1523426784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -651,7 +651,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1886019952"/>
+        <c:crossAx val="1523418624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -659,7 +659,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1886019952"/>
+        <c:axId val="1523418624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -766,7 +766,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1886015600"/>
+        <c:crossAx val="1523426784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -882,7 +882,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -972,7 +971,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1044,11 +1042,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1886019408"/>
-        <c:axId val="-1886018864"/>
+        <c:axId val="1523416992"/>
+        <c:axId val="1523422432"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1886019408"/>
+        <c:axId val="1523416992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1091,7 +1089,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1886018864"/>
+        <c:crossAx val="1523422432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1099,7 +1097,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1886018864"/>
+        <c:axId val="1523422432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1145,7 +1143,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1206,7 +1203,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1886019408"/>
+        <c:crossAx val="1523416992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2334,7 +2331,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="187" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="187" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="11" orientation="landscape" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -2401,7 +2398,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="6177243" cy="3774982"/>
+    <xdr:ext cx="6183610" cy="3779439"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Diagramm 1"/>
@@ -2716,8 +2713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F98"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="O56" sqref="O56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3698,7 +3695,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>